<commit_message>
transformaciones de log hechas
</commit_message>
<xml_diff>
--- a/archivos_entrad/Log-Vuelos.xlsx
+++ b/archivos_entrad/Log-Vuelos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="62">
   <si>
     <t>tipo vuelo</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t xml:space="preserve">28º  Viento del NO salimos por 04 de LETD. Vamos a Robledillo y sin traficos entramos por 01 , con viento cruzado. Hacemos un primera pasada baja, Luego 2 tomas con cruzado y terminamos con 2 tomas por la cruzada de LERM. Volvemos a LETD y hacemos 5 tomas, 2 con resbale. No sale todo muy bien, pero así se aprende. Si no lo veo claro tengo que tomar yo la decisión de motor y al aire. </t>
+  </si>
+  <si>
+    <t>29º  Nigun viento Cavok. 7 tomas 3 con resbale en LERM. La segunda mitad del vuelo como suelta. Buenas sensaciones</t>
   </si>
 </sst>
 </file>
@@ -223,12 +226,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -237,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -261,6 +270,19 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -608,19 +630,19 @@
       </c>
       <c r="M2" s="7">
         <f>SUM(I2:I50)</f>
-        <v>1.364583333</v>
+        <v>1.40625</v>
       </c>
       <c r="N2" s="7">
         <f>SUM(L2:L50)</f>
-        <v>1.166666667</v>
+        <v>1.208333333</v>
       </c>
       <c r="O2" s="8">
         <f>COUNTA(A2:A50)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P2" s="8">
         <f>max(F7:F50)-min(F7:F50)</f>
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="Q2" s="8">
         <f t="shared" ref="Q2:Q50" si="3">IF(A2="I",1,0)</f>
@@ -628,15 +650,15 @@
       </c>
       <c r="R2" s="8">
         <f>sum(Q2:Q50)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S2" s="8">
         <f>P2/HOUR(N2) + MINUTE(N2)/60</f>
-        <v>107.25</v>
+        <v>87.2</v>
       </c>
       <c r="T2" s="9">
         <f>HOUR(N2)*150</f>
-        <v>600</v>
+        <v>750</v>
       </c>
     </row>
     <row r="3">
@@ -867,7 +889,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="4">
-        <v>45597.0</v>
+        <v>45606.0</v>
       </c>
       <c r="G8" s="5">
         <v>0.5208333333333334</v>
@@ -2054,18 +2076,48 @@
       </c>
     </row>
     <row r="36">
-      <c r="I36" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K36" s="6"/>
+      <c r="A36" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="14">
+        <v>46033.0</v>
+      </c>
+      <c r="G36" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="H36" s="15">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="I36" s="16">
+        <f t="shared" si="1"/>
+        <v>0.04166666667</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K36" s="17"/>
       <c r="L36" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.04166666667</v>
       </c>
       <c r="Q36" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="37">
@@ -2281,7 +2333,7 @@
     <row r="132">
       <c r="L132" s="6">
         <f>SUM(L2:L131)</f>
-        <v>1.166666667</v>
+        <v>1.208333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>